<commit_message>
Choosen the structure of the ALU Opcode
More information inside the excel file
</commit_message>
<xml_diff>
--- a/Execute_Stage/ALU_control_signals.xlsx
+++ b/Execute_Stage/ALU_control_signals.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="124">
   <si>
     <t>ADDI</t>
   </si>
@@ -224,13 +224,175 @@
   </si>
   <si>
     <t>0100</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>0011</t>
+  </si>
+  <si>
+    <t>SLL</t>
+  </si>
+  <si>
+    <t>SRL</t>
+  </si>
+  <si>
+    <t>SRA</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>Primo appunto: l'adder, il logicals e il comparatore non sono mai attivi insieme, quindi ho bisogno di due bit per poter identificare quale componente tra loro sta lavorando. Potrei proprio scegliere UUW 2-bit</t>
+  </si>
+  <si>
+    <t>Occupati i primi due bit, adesso c'è da gestire gli altri 4, i quali si adattano perfettamente all'OPCODE di logicals e del comparator</t>
+  </si>
+  <si>
+    <t>Analizziamo il significato dell'OPCODE per entrambi i componenti, in modo tale da scegliere dove piazzare il Cin dell'adder ed il BS_Amount dello shifter</t>
+  </si>
+  <si>
+    <t>OPCODE</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>LOGICALS</t>
+  </si>
+  <si>
+    <t>CMP</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>XOR</t>
+  </si>
+  <si>
+    <t>SLTUI/SLTU</t>
+  </si>
+  <si>
+    <t>SGTUI/SGTU</t>
+  </si>
+  <si>
+    <t>SLEUI/SLEU</t>
+  </si>
+  <si>
+    <t>SGEUI/SGEU</t>
+  </si>
+  <si>
+    <t>SEQI/SEQ</t>
+  </si>
+  <si>
+    <t>SNEI/SNE</t>
+  </si>
+  <si>
+    <t>SLTI/SLT</t>
+  </si>
+  <si>
+    <t>SGTI/SGT</t>
+  </si>
+  <si>
+    <t>SLEI/SLE</t>
+  </si>
+  <si>
+    <t>SGEI/SGE</t>
+  </si>
+  <si>
+    <t>Bisogna agire nelle zone verdi!</t>
+  </si>
+  <si>
+    <t>Candidati papapibli per la manovrazione sono 1100, 1101, 1111.</t>
+  </si>
+  <si>
+    <t>Anche se (!!!), poiché logicals spende molto meno del comparatore,</t>
+  </si>
+  <si>
+    <t>possiamo agire anche in situazioni in cui l'opcode farebbe lavorare solo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logicals e non il comparatore. Quindi ulteriori candidati sono </t>
+  </si>
+  <si>
+    <t>0001, 0110, 0111.</t>
+  </si>
+  <si>
+    <t>In definitiva:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analizziamo dove avviene il minor cambio di bit tra un </t>
+  </si>
+  <si>
+    <t>numero e l'altro -------&gt;</t>
+  </si>
+  <si>
+    <t>Coppie candidate</t>
+  </si>
+  <si>
+    <t>0110 &amp; 0111</t>
+  </si>
+  <si>
+    <t>0111 &amp; 1111</t>
+  </si>
+  <si>
+    <t>1100 &amp; 1101</t>
+  </si>
+  <si>
+    <t>1101 &amp; 1111</t>
+  </si>
+  <si>
+    <t>&lt;- più intuitivo, ma più efficace?</t>
+  </si>
+  <si>
+    <t>UUW(1)</t>
+  </si>
+  <si>
+    <t>UUW(0)</t>
+  </si>
+  <si>
+    <t>Cin</t>
+  </si>
+  <si>
+    <t>BS_Opcode(1)</t>
+  </si>
+  <si>
+    <t>BS_Opcode(0)</t>
+  </si>
+  <si>
+    <t>(Solo per Shifter &amp; adder) !!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,8 +415,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +441,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,7 +500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -294,6 +513,19 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -599,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:O95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,37 +849,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="6" t="s">
         <v>57</v>
       </c>
     </row>
@@ -655,6 +889,25 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9"/>
       <c r="I2" s="1" t="s">
         <v>58</v>
       </c>
@@ -675,6 +928,25 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9"/>
       <c r="I3" s="3" t="s">
         <v>58</v>
       </c>
@@ -695,6 +967,25 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9"/>
       <c r="I4" s="3" t="s">
         <v>58</v>
       </c>
@@ -715,6 +1006,25 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9"/>
       <c r="I5" s="3" t="s">
         <v>58</v>
       </c>
@@ -735,6 +1045,25 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9"/>
       <c r="I6" s="3" t="s">
         <v>58</v>
       </c>
@@ -755,6 +1084,25 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9"/>
       <c r="I7" s="3" t="s">
         <v>58</v>
       </c>
@@ -775,6 +1123,25 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9"/>
       <c r="I8" s="3" t="s">
         <v>58</v>
       </c>
@@ -795,7 +1162,25 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="B9" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9"/>
       <c r="I9" s="2" t="s">
         <v>66</v>
       </c>
@@ -816,6 +1201,25 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9"/>
       <c r="I10" s="2" t="s">
         <v>67</v>
       </c>
@@ -836,6 +1240,25 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9"/>
       <c r="I11" s="3" t="s">
         <v>58</v>
       </c>
@@ -856,6 +1279,25 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9"/>
       <c r="I12" s="2" t="s">
         <v>63</v>
       </c>
@@ -876,6 +1318,25 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9"/>
       <c r="I13" s="2" t="s">
         <v>68</v>
       </c>
@@ -896,6 +1357,25 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9"/>
       <c r="I14" s="3" t="s">
         <v>58</v>
       </c>
@@ -916,6 +1396,25 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9"/>
       <c r="I15" s="3" t="s">
         <v>58</v>
       </c>
@@ -925,375 +1424,1807 @@
       <c r="K15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="4"/>
+      <c r="L15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="4"/>
+      <c r="B16" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="4"/>
+      <c r="B17" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="4"/>
+      <c r="B18" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="4"/>
+      <c r="B19" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="4"/>
+      <c r="B20" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="4"/>
+      <c r="B21" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="4"/>
+      <c r="B22" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="4"/>
+      <c r="B23" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="4"/>
+      <c r="B24" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9"/>
+      <c r="I24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="4"/>
+      <c r="B25" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="9"/>
+      <c r="I25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9"/>
+      <c r="I28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="4"/>
+      <c r="B29" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="4"/>
+      <c r="B30" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="4"/>
+      <c r="B31" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="4"/>
+      <c r="B32" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="4"/>
+      <c r="B33" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="4"/>
+      <c r="B34" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="4"/>
+      <c r="B35" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="4"/>
+      <c r="B36" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="4"/>
+      <c r="B37" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="4"/>
+      <c r="B38" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>34</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="4"/>
+      <c r="B39" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="I39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>35</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="4"/>
+      <c r="B40" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40" s="9"/>
+      <c r="I40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="4"/>
+      <c r="B41" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>37</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="4"/>
+      <c r="B42" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="4"/>
+      <c r="B43" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" s="9"/>
+      <c r="I43" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>39</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="4"/>
+      <c r="B44" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44" s="9"/>
+      <c r="I44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>40</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="4"/>
+      <c r="B45" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45" s="9"/>
+      <c r="I45" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F46" s="12"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="4"/>
+      <c r="K46" s="4"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="4"/>
+      <c r="B47" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" s="12">
+        <v>1</v>
+      </c>
+      <c r="G47" s="12">
+        <v>1</v>
+      </c>
+      <c r="H47" s="9"/>
+      <c r="I47" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="4"/>
+      <c r="B48" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="12">
+        <v>1</v>
+      </c>
+      <c r="G48" s="12">
+        <v>1</v>
+      </c>
+      <c r="H48" s="9"/>
+      <c r="I48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>43</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="4"/>
+      <c r="B49" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" s="12">
+        <v>0</v>
+      </c>
+      <c r="G49" s="12">
+        <v>1</v>
+      </c>
+      <c r="H49" s="9"/>
+      <c r="I49" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>44</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="4"/>
+      <c r="B50" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" s="12">
+        <v>0</v>
+      </c>
+      <c r="G50" s="12">
+        <v>1</v>
+      </c>
+      <c r="H50" s="9"/>
+      <c r="I50" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>45</v>
       </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="4"/>
+      <c r="B51" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" s="12">
+        <v>0</v>
+      </c>
+      <c r="G51" s="12">
+        <v>1</v>
+      </c>
+      <c r="H51" s="9"/>
+      <c r="I51" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>46</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="4"/>
+      <c r="B52" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" s="12">
+        <v>0</v>
+      </c>
+      <c r="G52" s="12">
+        <v>1</v>
+      </c>
+      <c r="H52" s="9"/>
+      <c r="I52" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" t="s">
+        <v>88</v>
+      </c>
+      <c r="E63" t="s">
+        <v>89</v>
+      </c>
+      <c r="J63">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="E64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="11"/>
+      <c r="E66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" s="11"/>
+      <c r="E67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="E68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="E69" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C70" t="s">
+        <v>92</v>
+      </c>
+      <c r="E70" s="11"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E71" s="11"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" t="s">
+        <v>90</v>
+      </c>
+      <c r="E72" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E73" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="11"/>
+      <c r="E74" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75" s="11"/>
+      <c r="E75" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="I76" t="s">
+        <v>103</v>
+      </c>
+      <c r="K76" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+      <c r="K77" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" t="s">
+        <v>91</v>
+      </c>
+      <c r="E78" s="11"/>
+      <c r="K78" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="8"/>
+      <c r="K79" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K80" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
+        <v>109</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L82" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N82" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O82" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I83" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="7"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="7"/>
+    </row>
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>110</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J84">
+        <v>2</v>
+      </c>
+      <c r="K84" s="7"/>
+      <c r="L84" s="7"/>
+      <c r="M84" s="7"/>
+      <c r="N84" s="7"/>
+      <c r="O84" s="7"/>
+    </row>
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>111</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J85">
+        <v>2</v>
+      </c>
+      <c r="K85" s="9">
+        <v>1</v>
+      </c>
+      <c r="L85" s="7"/>
+      <c r="M85" s="7"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="7"/>
+    </row>
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I86" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J86">
+        <v>3</v>
+      </c>
+      <c r="K86">
+        <v>2</v>
+      </c>
+      <c r="L86">
+        <v>3</v>
+      </c>
+      <c r="M86" s="7"/>
+      <c r="N86" s="7"/>
+      <c r="O86" s="7"/>
+    </row>
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I87" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J87">
+        <v>2</v>
+      </c>
+      <c r="K87">
+        <v>3</v>
+      </c>
+      <c r="L87">
+        <v>2</v>
+      </c>
+      <c r="M87" s="9">
+        <v>1</v>
+      </c>
+      <c r="N87" s="7"/>
+      <c r="O87" s="7"/>
+    </row>
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I88" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J88">
+        <v>3</v>
+      </c>
+      <c r="K88">
+        <v>2</v>
+      </c>
+      <c r="L88" s="9">
+        <v>1</v>
+      </c>
+      <c r="M88">
+        <v>2</v>
+      </c>
+      <c r="N88" s="9">
+        <v>1</v>
+      </c>
+      <c r="O88" s="7"/>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N89" s="12"/>
+    </row>
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B92" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C92" s="10"/>
+    </row>
+    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B93" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C93" s="10"/>
+    </row>
+    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B94" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C94" s="10"/>
+      <c r="E94" t="s">
+        <v>117</v>
+      </c>
+      <c r="I94" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="J94" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="K94" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="L94" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="M94" s="15">
+        <v>0</v>
+      </c>
+      <c r="N94" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B95" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C95" s="10"/>
+      <c r="E95" s="6" t="s">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ALU v 0.4 ready for syn
Changed a little bit the structure of the alu opcode, because befaore I
couldn't distinguish between signed and unsigned adds and subs. All
proposed tests have been passed. Ready for Synopsys' step.
</commit_message>
<xml_diff>
--- a/Execute_Stage/ALU_control_signals.xlsx
+++ b/Execute_Stage/ALU_control_signals.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="125">
   <si>
     <t>ADDI</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>(Solo per Shifter &amp; adder) !!!</t>
+  </si>
+  <si>
+    <t>SGN/usgn</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -486,6 +489,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -500,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -526,6 +535,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -833,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="L97" sqref="L97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,8 +911,8 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
+      <c r="F2" s="17">
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -979,8 +989,8 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="F4" s="17">
+        <v>1</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1954,8 +1964,8 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29">
-        <v>0</v>
+      <c r="F29" s="17">
+        <v>1</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -2032,8 +2042,8 @@
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31">
-        <v>0</v>
+      <c r="F31" s="17">
+        <v>1</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -3210,8 +3220,8 @@
       <c r="L94" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="M94" s="15">
-        <v>0</v>
+      <c r="M94" s="15" t="s">
+        <v>124</v>
       </c>
       <c r="N94" s="14" t="s">
         <v>120</v>

</xml_diff>